<commit_message>
fill out command table, do extra credit
</commit_message>
<xml_diff>
--- a/questions/Client Command Table A9.xlsx
+++ b/questions/Client Command Table A9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjornnelson/SimplicityStudio/v5_workspace/ecen5823-assignment7-bjornhnelson/questions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjornnelson/SimplicityStudio/v5_workspace/ecen5823-assignment9-bjornhnelson/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B0EAC-64D8-AB4F-9F9E-6485E9369B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD514BD-967D-1346-B568-2BD1EC6E2BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="98">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -161,12 +161,6 @@
     <t>Set the default Bluetooth connection parameters.</t>
   </si>
   <si>
-    <t>scan interval, scan window</t>
-  </si>
-  <si>
-    <t>min/max interval, latency, timeout</t>
-  </si>
-  <si>
     <t>Start the GAP discovery procedure to scan for advertising devices on the specified scanning PHY or to perform a device discovery.</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>characteristic handle (sl_bt_evt_gatt_characteristic-&gt;characteristic)</t>
   </si>
   <si>
-    <t>characteristic value (sl_bt_evt_gatt_characteristic_value-&gt;value)</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>sl_bt_connection_open()</t>
   </si>
   <si>
-    <t>packet type, address, address type</t>
-  </si>
-  <si>
     <t>Connect to an advertising device with the specified initiating PHY on which connectable advertisements on primary advertising channels are received.</t>
   </si>
   <si>
@@ -273,9 +261,6 @@
     <t>Discover all characteristics of a GATT service in a remote GATT database having the specified UUID.</t>
   </si>
   <si>
-    <t>If indication is from temperature service, call LCD display function to show latest temp value</t>
-  </si>
-  <si>
     <t>Various API calls to initialize the client</t>
   </si>
   <si>
@@ -285,12 +270,6 @@
     <t>Advance state machine to discovering service state, call sl_bt_gatt_discover_primary_services_by_uuid() before doing so</t>
   </si>
   <si>
-    <t>Case 1: When service matching UUID is found (in discovering service state), call sl_bt_gatt_discover_characteristics_by_uuid() and advance state machine to discovering characteristic state</t>
-  </si>
-  <si>
-    <t>Case 2: When characteristic matching UUID is found (in discovering characteristic state), call sl_bt_gatt_set_characteristic_notification() and advance state machine to receiving indications state</t>
-  </si>
-  <si>
     <t>Case 3: When in receiving indications state, do nothing (keep receiving indications)</t>
   </si>
   <si>
@@ -307,6 +286,90 @@
   </si>
   <si>
     <t>DISPLAY_ROW_CONNECTION - discovering, DISPLAY_ROW_NAME - client, DISPLAY_ROW_BTADDR - client address, DISPLAY_ROW_ASSIGNMENT - A7</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_system_external_signal_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_confirm_passkey_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_bonded_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_bonding_failed_id</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_delete_bondings()</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_configure()</t>
+  </si>
+  <si>
+    <t>Delete previous bonding info</t>
+  </si>
+  <si>
+    <t>Set up security manager</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_read_characteristic_value()</t>
+  </si>
+  <si>
+    <t>Call when PB1 pressed and PB0 not pressed</t>
+  </si>
+  <si>
+    <t>Call when both PB0 and PB1 pressed</t>
+  </si>
+  <si>
+    <t>Show passkey message</t>
+  </si>
+  <si>
+    <t>Show bonded status</t>
+  </si>
+  <si>
+    <t>Update LCD</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_passkey_confirm()</t>
+  </si>
+  <si>
+    <t>Call in secure pairing process</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_increase_security()</t>
+  </si>
+  <si>
+    <t>Call when pushing PB1 for first time to initiate secure pairing</t>
+  </si>
+  <si>
+    <t>Process indications and read events, updates LCD to show HTM and PB data</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_9 - Button Status</t>
+  </si>
+  <si>
+    <t>Case 1: When service matching UUID is found for HTM or PB, call sl_bt_gatt_discover_characteristics_by_uuid() and advance state machine to corresponding discovering characteristic state</t>
+  </si>
+  <si>
+    <t>Case 2: When both HTM and PB characteristics matching UUIDs are found, call sl_bt_gatt_set_characteristic_notification() and advance state machine to receiving indications state</t>
+  </si>
+  <si>
+    <t>Call twice, once for HTM service and once for PB service</t>
+  </si>
+  <si>
+    <t>Indicates a request for passkey display and confirmation by the user.</t>
+  </si>
+  <si>
+    <t>Triggered after the pairing or bonding procedure is successfully completed.</t>
+  </si>
+  <si>
+    <t>This event is triggered if the pairing or bonding procedure fails.</t>
+  </si>
+  <si>
+    <t>Indicates that the external signals have been received.</t>
+  </si>
+  <si>
+    <t>characteristic value</t>
   </si>
 </sst>
 </file>
@@ -405,7 +468,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +481,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -509,11 +578,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -605,6 +689,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,22 +789,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>539658</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>74041</xdr:rowOff>
+      <xdr:colOff>605693</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>78154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1134533</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>125345</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>521620</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>58616</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A94616ED-66C4-EE40-9F87-96D3BA587628}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{631C2027-98DE-F34D-9CF6-8D023C78AA31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -727,8 +820,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19386458" y="2495508"/>
-          <a:ext cx="8113275" cy="5266770"/>
+          <a:off x="19440770" y="1914769"/>
+          <a:ext cx="19923312" cy="6584462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1818,10 +1911,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1872,7 +1965,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -1928,169 +2021,169 @@
         <v>10</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="25"/>
       <c r="H7" s="32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="15"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="23" t="s">
-        <v>37</v>
-      </c>
+      <c r="F10" s="13"/>
       <c r="G10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>43</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>15</v>
-      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24" t="s">
-        <v>68</v>
+      <c r="B13" s="4"/>
+      <c r="C13" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="16" t="s">
-        <v>49</v>
-      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="24" t="s">
-        <v>48</v>
-      </c>
+      <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="16"/>
+      <c r="B15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>41</v>
+      <c r="B17" s="4"/>
+      <c r="C17" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="D17" s="16"/>
-      <c r="E17" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="16"/>
+      <c r="G17" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -2099,38 +2192,36 @@
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>67</v>
-      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="E19" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>44</v>
+      <c r="B20" s="17"/>
+      <c r="C20" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="D20" s="16"/>
-      <c r="E20" s="24" t="s">
-        <v>56</v>
-      </c>
+      <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="27" t="s">
-        <v>45</v>
+      <c r="G20" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="H20" s="16"/>
     </row>
@@ -2141,200 +2232,198 @@
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="G21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>21</v>
+      <c r="B23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="21" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="29" t="s">
-        <v>39</v>
-      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="16"/>
+      <c r="B25" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F25" s="16"/>
-      <c r="G25" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>72</v>
-      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>23</v>
-      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="24" t="s">
-        <v>46</v>
-      </c>
+      <c r="E27" s="24"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="20" t="s">
-        <v>24</v>
+      <c r="G27" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>69</v>
+      <c r="G28" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" s="37" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>70</v>
-      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+      <c r="B30" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F30" s="16"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24" t="s">
-        <v>71</v>
+      <c r="G30" s="27"/>
+      <c r="H30" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="16"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
@@ -2346,49 +2435,264 @@
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8" ht="65.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="E37" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="C38" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="29" t="s">
+        <v>37</v>
+      </c>
       <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="16"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="18"/>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" s="28"/>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="1:8" ht="65.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>